<commit_message>
Append excel, more info
</commit_message>
<xml_diff>
--- a/jobs.xlsx
+++ b/jobs.xlsx
@@ -6,17 +6,17 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="NoFluff" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <charset val="238"/>
@@ -32,6 +32,15 @@
       <color theme="10"/>
       <sz val="11"/>
       <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="238"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -56,9 +65,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -437,366 +449,368 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C173"/>
+  <dimension ref="A1:E210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="109.140625" customWidth="1" min="1" max="1"/>
+    <col width="67.28515625" customWidth="1" min="1" max="1"/>
     <col width="46.5703125" customWidth="1" min="2" max="2"/>
-    <col width="49.42578125" customWidth="1" min="3" max="3"/>
+    <col width="33.28515625" customWidth="1" min="3" max="3"/>
+    <col width="29.7109375" customWidth="1" min="4" max="4"/>
+    <col width="22.28515625" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Tytuł</t>
+    <row r="1" customFormat="1" s="2">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>LINK</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>OPIS</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>FIRMA</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>ZAROBKI</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>LOKALIZACJA</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/qa-automation-engineer-c--shiji-poland-remote</t>
-        </is>
+      <c r="A2">
+        <f>HYPERLINK("https://nofluffjobs.com/pl/job/senior-mobile-qa-automation-engineer-beekeeper-remote", "https://nofluffjobs.com/pl/job/senior-mobile-qa-automation-engineer-beekeeper-remote")</f>
+        <v/>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[' QA Automation Engineer (C#)  ']</t>
+          <t xml:space="preserve"> Senior Mobile QA Automation Engineer </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[' Shiji Poland ']</t>
+          <t xml:space="preserve"> Beekeeper AG </t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 17500  – 26666  PLN</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Zdalnie   +1 </t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/remote-senior-software-tester-ibm-bto</t>
-        </is>
+      <c r="A3">
+        <f>HYPERLINK("https://nofluffjobs.com/pl/job/qa-engineer-grape-up-remote-2", "https://nofluffjobs.com/pl/job/qa-engineer-grape-up-remote-2")</f>
+        <v/>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[' Remote Senior Software Tester ']</t>
+          <t xml:space="preserve"> QA Engineer </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>[' IBM BTO ']</t>
+          <t xml:space="preserve"> Grape Up </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12000  – 18000  PLN</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Zdalnie   +3 </t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/remote-test-engineer-mid-hyland</t>
-        </is>
+      <c r="A4">
+        <f>HYPERLINK("https://nofluffjobs.com/pl/job/senior-test-engineer-rpo-partners-gdansk", "https://nofluffjobs.com/pl/job/senior-test-engineer-rpo-partners-gdansk")</f>
+        <v/>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[' Remote Test Engineer (Mid) ']</t>
+          <t xml:space="preserve"> Senior Test Engineer </t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>[' Hyland ']</t>
+          <t xml:space="preserve"> RPO Partners Sp. z o.o. </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12000  – 23000  PLN</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Gdańsk  </t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/test-automation-engineer-ework-group-warszawa-5</t>
-        </is>
+      <c r="A5">
+        <f>HYPERLINK("https://nofluffjobs.com/pl/job/test-automation-engineer-sii-polska-remote-7", "https://nofluffjobs.com/pl/job/test-automation-engineer-sii-polska-remote-7")</f>
+        <v/>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[' Test Automation Engineer ']</t>
+          <t xml:space="preserve"> Test Automation Engineer </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[' Ework Group ']</t>
+          <t xml:space="preserve"> Sii Polska </t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 21840  – 25410  PLN</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Zdalnie   +5 </t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/senior-qa-automation-engineer-codibly-remote-1</t>
-        </is>
+      <c r="A6">
+        <f>HYPERLINK("https://nofluffjobs.com/pl/job/tester-automatyzujacy-remote-link-group", "https://nofluffjobs.com/pl/job/tester-automatyzujacy-remote-link-group")</f>
+        <v/>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[' Senior QA Automation Engineer ']</t>
+          <t xml:space="preserve"> Tester Automatyzujący - Remote </t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>[' Codibly ']</t>
+          <t xml:space="preserve"> Link Group </t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16800  – 21840  PLN</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Zdalnie   +1 </t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/remote-mid-qa-engineer-tester-crehler</t>
-        </is>
+      <c r="A7">
+        <f>HYPERLINK("https://nofluffjobs.com/pl/job/remote-automation-qa-with-python-aws-valtech", "https://nofluffjobs.com/pl/job/remote-automation-qa-with-python-aws-valtech")</f>
+        <v/>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[' Remote Mid QA Engineer / Tester ']</t>
+          <t xml:space="preserve"> Remote Automation QA with Python&amp;AWS  </t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>[' CREHLER Sp. z o.o. ']</t>
+          <t xml:space="preserve"> Valtech </t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 18597  – 27896  PLN</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Zdalnie  </t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/tester-manualny-avenga-warszawa</t>
-        </is>
+      <c r="A8">
+        <f>HYPERLINK("https://nofluffjobs.com/pl/job/senior-qa-engineer-focal-systems-remote", "https://nofluffjobs.com/pl/job/senior-qa-engineer-focal-systems-remote")</f>
+        <v/>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[' Tester manualny ']</t>
+          <t xml:space="preserve"> Senior QA Engineer </t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[' AVENGA ']</t>
+          <t xml:space="preserve"> Focal Systems </t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 25000  – 35000  PLN</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Zdalnie  </t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/mid-fullstack-developer-java-react-link-group-warszawa</t>
-        </is>
+      <c r="A9">
+        <f>HYPERLINK("https://nofluffjobs.com/pl/job/senior-software-tester-macrix-technology-group-remote-1", "https://nofluffjobs.com/pl/job/senior-software-tester-macrix-technology-group-remote-1")</f>
+        <v/>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[' Mid Fullstack Developer Java / React ']</t>
+          <t xml:space="preserve"> Senior Software Tester </t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>[' Link Group ']</t>
+          <t xml:space="preserve"> Macrix Technology Group </t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 14500  – 24000  PLN</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Zdalnie   +1 </t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/test-automation-engineer-with-net-bestmix-software-wroclaw-1</t>
-        </is>
+      <c r="A10">
+        <f>HYPERLINK("https://nofluffjobs.com/pl/job/mid-senior-network-engineer-with-python-codilime-remote", "https://nofluffjobs.com/pl/job/mid-senior-network-engineer-with-python-codilime-remote")</f>
+        <v/>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[' Test Automation Engineer with .NET ']</t>
+          <t xml:space="preserve"> Mid/Senior Network Engineer with Python </t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[' Bestmix Software ']</t>
+          <t xml:space="preserve"> CodiLime </t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 18000  – 31000  PLN</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Zdalnie   +16 </t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/qa-engineer-comscore-remote</t>
-        </is>
+      <c r="A11">
+        <f>HYPERLINK("https://nofluffjobs.com/pl/job/qa-engineer-link-group-warszawa-2", "https://nofluffjobs.com/pl/job/qa-engineer-link-group-warszawa-2")</f>
+        <v/>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[' QA Engineer ']</t>
+          <t xml:space="preserve">  QA Engineer  </t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>[' ComScore ']</t>
+          <t xml:space="preserve"> Link Group </t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28000  – 35000  PLN</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Warszawa   +6 </t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/qa-engineer-adjutor-remote-1</t>
-        </is>
+      <c r="A12">
+        <f>HYPERLINK("https://nofluffjobs.com/pl/job/mid-senior-qa-automation-engineer-andea-solutions-remote-1", "https://nofluffjobs.com/pl/job/mid-senior-qa-automation-engineer-andea-solutions-remote-1")</f>
+        <v/>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[' QA Engineer ']</t>
+          <t xml:space="preserve"> Mid/Senior QA Automation Engineer </t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>[' Adjutor ']</t>
+          <t xml:space="preserve"> Andea Solutions Sp. z o.o. </t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12000  – 20000  PLN</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Zdalnie  </t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/quality-assurance-specialist-hitachi-energy-krakow</t>
-        </is>
+      <c r="A13">
+        <f>HYPERLINK("https://nofluffjobs.com/pl/job/qa-engineer-march-networks-poland-gliwice", "https://nofluffjobs.com/pl/job/qa-engineer-march-networks-poland-gliwice")</f>
+        <v/>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[' Quality Assurance Specialist ']</t>
+          <t xml:space="preserve"> QA Engineer </t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>[' Hitachi Energy ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/koordynator-testow-connectis--warsaw</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>[' Koordynator testów ']</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>[' Connectis_ ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/mid-senior-qa-automation-engineer-andea-solutions-remote-1</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>[' Mid/Senior QA Automation Engineer ']</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>[' Andea Solutions Sp. z o.o. ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/qa-automation-engineer-javascript-avenga-remote-1</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>[' QA Automation Engineer (JavaScript) ']</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>[' Avenga ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/qa-engineer-march-networks-poland-gliwice</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>[' QA Engineer ']</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>[' March Networks Poland Sp. z o.o ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/manual-tester-avenga-wroclaw-5</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>[' Manual Tester ']</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>[' AVENGA ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/qa-automation-engineer-i-hl-tech-remote</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>[' QA Automation Engineer I ']</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>[' HL Tech ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/tester-automatyzujacy-avenga-warszawa-2</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>[' Tester Automatyzujący ']</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>[' AVENGA ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>https://nofluffjobs.com/pl/job/quality-software-engineer-avenga-remote</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>[' Quality Software Engineer  ']</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>[' Avenga ']</t>
-        </is>
-      </c>
-    </row>
+          <t xml:space="preserve"> March Networks Poland Sp. z o.o </t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8000  – 12000  PLN</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Gliwice  </t>
+        </is>
+      </c>
+    </row>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
     <row r="22"/>
     <row r="23"/>
     <row r="24"/>
@@ -948,10 +962,48 @@
     <row r="170"/>
     <row r="171"/>
     <row r="172"/>
-    <row r="173">
-      <c r="A173" s="1" t="n"/>
+    <row r="173"/>
+    <row r="174"/>
+    <row r="175"/>
+    <row r="176"/>
+    <row r="177"/>
+    <row r="178"/>
+    <row r="179"/>
+    <row r="180"/>
+    <row r="181"/>
+    <row r="182"/>
+    <row r="183"/>
+    <row r="184"/>
+    <row r="185"/>
+    <row r="186"/>
+    <row r="187"/>
+    <row r="188"/>
+    <row r="189"/>
+    <row r="190"/>
+    <row r="191"/>
+    <row r="192"/>
+    <row r="193"/>
+    <row r="194"/>
+    <row r="195"/>
+    <row r="196"/>
+    <row r="197"/>
+    <row r="198"/>
+    <row r="199"/>
+    <row r="200"/>
+    <row r="201"/>
+    <row r="202"/>
+    <row r="203"/>
+    <row r="204"/>
+    <row r="205"/>
+    <row r="206"/>
+    <row r="207"/>
+    <row r="208"/>
+    <row r="209"/>
+    <row r="210">
+      <c r="A210" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>